<commit_message>
update des schémas + pieces en stock. Version finale
le tableau des pieces en stock est out of date. les schémas sont
fonctionnels
</commit_message>
<xml_diff>
--- a/Pieces/Tableau_pieces_en_stock.xlsx
+++ b/Pieces/Tableau_pieces_en_stock.xlsx
@@ -5,23 +5,23 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\GitHub\243-510-A15\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mathieu\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8145"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
     <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511" iterateDelta="1E-4"/>
+  <calcPr calcId="162913" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="125">
   <si>
     <t>INVENTAIRE DES PIÈCES DISPONIBLES</t>
   </si>
@@ -233,23 +233,176 @@
     <t>Alkaline</t>
   </si>
   <si>
-    <t>Total</t>
-  </si>
-  <si>
     <t>quantité utilisé</t>
   </si>
   <si>
-    <t>PAR AGATHE</t>
-  </si>
-  <si>
-    <t>Jumper</t>
+    <t>PIC 18f46J50</t>
+  </si>
+  <si>
+    <t>microchip</t>
+  </si>
+  <si>
+    <t>PIC18F45J50-I/PT</t>
+  </si>
+  <si>
+    <t>Switch slide</t>
+  </si>
+  <si>
+    <t>JS202011SCQN</t>
+  </si>
+  <si>
+    <t>micro USB-B</t>
+  </si>
+  <si>
+    <t>10118192-0001LF</t>
+  </si>
+  <si>
+    <t>FCI</t>
+  </si>
+  <si>
+    <t>YAGEO</t>
+  </si>
+  <si>
+    <t>CC0805ZKY5V6BB106</t>
+  </si>
+  <si>
+    <t>Abracon LLC</t>
+  </si>
+  <si>
+    <t>AB26TRQ-32.768KHZ-T</t>
+  </si>
+  <si>
+    <t>Écran</t>
+  </si>
+  <si>
+    <t>RC0805JR-0736KL</t>
+  </si>
+  <si>
+    <t>Chargeur</t>
+  </si>
+  <si>
+    <t>MCP73871-2CCI/ML</t>
+  </si>
+  <si>
+    <t>Régulateur</t>
+  </si>
+  <si>
+    <t>LM3671MF-3.3/NOPB</t>
+  </si>
+  <si>
+    <t>PTS645SM43SMTR92 LFS</t>
+  </si>
+  <si>
+    <t>10uF</t>
+  </si>
+  <si>
+    <t>3,3V</t>
+  </si>
+  <si>
+    <t>CL21F104ZBCNNNC</t>
+  </si>
+  <si>
+    <t>RC0805JR-07110KL</t>
+  </si>
+  <si>
+    <t>110k 5%</t>
+  </si>
+  <si>
+    <t>Stackpole</t>
+  </si>
+  <si>
+    <t>RNCP0805FTD40k2</t>
+  </si>
+  <si>
+    <t>40,2k 1%</t>
+  </si>
+  <si>
+    <t>RNCP0805FTD10k0</t>
+  </si>
+  <si>
+    <t>10k 1%</t>
+  </si>
+  <si>
+    <t>Bobine</t>
+  </si>
+  <si>
+    <t>TDK corporation</t>
+  </si>
+  <si>
+    <t>MLZ2012A2R2M</t>
+  </si>
+  <si>
+    <t>2,2uH 650mA 150ohm</t>
+  </si>
+  <si>
+    <t>RNCP0805FTD2k00</t>
+  </si>
+  <si>
+    <t>2k 1%</t>
+  </si>
+  <si>
+    <t>CC0805ZRY5V6BB475</t>
+  </si>
+  <si>
+    <t>4,7uF</t>
+  </si>
+  <si>
+    <t>RNCP0805FTD1k00</t>
+  </si>
+  <si>
+    <t>1k 1%</t>
+  </si>
+  <si>
+    <t>APT2012EC</t>
+  </si>
+  <si>
+    <t>rouge</t>
+  </si>
+  <si>
+    <t>APT2012SGC</t>
+  </si>
+  <si>
+    <t>vert</t>
+  </si>
+  <si>
+    <t>KEMET</t>
+  </si>
+  <si>
+    <t>L0603C3N9SRMST</t>
+  </si>
+  <si>
+    <t>JONATHAN</t>
+  </si>
+  <si>
+    <t>AVX</t>
+  </si>
+  <si>
+    <t>HLC025R6BTTR</t>
+  </si>
+  <si>
+    <t>EPCOS</t>
+  </si>
+  <si>
+    <t>B82496C3829J</t>
+  </si>
+  <si>
+    <t>2 for JONATHAN</t>
+  </si>
+  <si>
+    <t>(1 brulé)</t>
+  </si>
+  <si>
+    <t>36k 5%</t>
+  </si>
+  <si>
+    <t>(2 jettés)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -274,16 +427,29 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -307,6 +473,72 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color auto="1"/>
       </left>
@@ -317,24 +549,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -350,21 +569,394 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="11">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -375,6 +967,23 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A5:H50" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1" tableBorderDxfId="10">
+  <autoFilter ref="A5:H50"/>
+  <tableColumns count="8">
+    <tableColumn id="1" name="Pièces" dataDxfId="9"/>
+    <tableColumn id="2" name="Manifacturer" dataDxfId="8"/>
+    <tableColumn id="3" name="Manifacturer Part" dataDxfId="7"/>
+    <tableColumn id="4" name="Caractéristiques" dataDxfId="6"/>
+    <tableColumn id="5" name="Prix unité" dataDxfId="5"/>
+    <tableColumn id="6" name="Quantité" dataDxfId="4"/>
+    <tableColumn id="7" name="Prix total/pièce" dataDxfId="3"/>
+    <tableColumn id="8" name="quantité utilisé" dataDxfId="2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -640,10 +1249,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J31"/>
+  <dimension ref="A1:J50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -654,7 +1263,7 @@
     <col min="5" max="5" width="10.5703125"/>
     <col min="6" max="6" width="10.42578125"/>
     <col min="7" max="7" width="15.85546875"/>
-    <col min="8" max="8" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15" customWidth="1"/>
     <col min="9" max="9" width="15.85546875"/>
     <col min="10" max="1025" width="10.5703125"/>
   </cols>
@@ -687,46 +1296,47 @@
       <c r="G3" s="2"/>
     </row>
     <row r="4" spans="1:10" ht="25.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
       <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="F5" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="11" t="s">
+      <c r="G5" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="9" t="s">
-        <v>71</v>
+      <c r="H5" s="22" t="s">
+        <v>70</v>
       </c>
       <c r="I5" s="4"/>
       <c r="J5" s="2"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="10" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="3" t="s">
@@ -746,12 +1356,12 @@
         <f t="shared" ref="G6:G25" si="0">E6*F6</f>
         <v>41.69</v>
       </c>
-      <c r="H6" s="3">
+      <c r="H6" s="11">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="10" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -771,12 +1381,15 @@
         <f t="shared" si="0"/>
         <v>9.02</v>
       </c>
-      <c r="H7" s="3">
-        <v>1</v>
+      <c r="H7" s="11">
+        <v>3</v>
+      </c>
+      <c r="I7" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="10" t="s">
         <v>14</v>
       </c>
       <c r="B8" s="3" t="s">
@@ -796,12 +1409,12 @@
         <f t="shared" si="0"/>
         <v>9.120000000000001</v>
       </c>
-      <c r="H8" s="3">
+      <c r="H8" s="11">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="15" t="s">
         <v>17</v>
       </c>
       <c r="B9" s="6" t="s">
@@ -823,12 +1436,12 @@
         <f t="shared" si="0"/>
         <v>2.04</v>
       </c>
-      <c r="H9" s="3">
-        <v>0.5</v>
+      <c r="H9" s="11">
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="15" t="s">
         <v>21</v>
       </c>
       <c r="B10" s="6" t="s">
@@ -848,12 +1461,12 @@
         <f t="shared" si="0"/>
         <v>6.82</v>
       </c>
-      <c r="H10" s="3">
+      <c r="H10" s="11">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="15" t="s">
         <v>24</v>
       </c>
       <c r="B11" s="6" t="s">
@@ -873,12 +1486,12 @@
         <f t="shared" si="0"/>
         <v>1.49</v>
       </c>
-      <c r="H11" s="3">
+      <c r="H11" s="11">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="15" t="s">
         <v>26</v>
       </c>
       <c r="B12" s="6" t="s">
@@ -898,12 +1511,12 @@
         <f t="shared" si="0"/>
         <v>9.84</v>
       </c>
-      <c r="H12" s="3">
-        <v>1</v>
+      <c r="H12" s="11">
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="15" t="s">
         <v>28</v>
       </c>
       <c r="B13" s="6" t="s">
@@ -923,12 +1536,12 @@
         <f t="shared" si="0"/>
         <v>6.9599999999999991</v>
       </c>
-      <c r="H13" s="3">
-        <v>1</v>
+      <c r="H13" s="11">
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="15" t="s">
         <v>30</v>
       </c>
       <c r="B14" s="6" t="s">
@@ -948,12 +1561,12 @@
         <f t="shared" si="0"/>
         <v>4.0500000000000007</v>
       </c>
-      <c r="H14" s="3">
-        <v>2</v>
+      <c r="H14" s="11">
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="15" t="s">
         <v>33</v>
       </c>
       <c r="B15" s="6" t="s">
@@ -975,12 +1588,12 @@
         <f t="shared" si="0"/>
         <v>7.0000000000000009</v>
       </c>
-      <c r="H15" s="12">
-        <v>2</v>
+      <c r="H15" s="18">
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="15" t="s">
         <v>33</v>
       </c>
       <c r="B16" s="6" t="s">
@@ -1002,12 +1615,12 @@
         <f t="shared" si="0"/>
         <v>7.0000000000000009</v>
       </c>
-      <c r="H16" s="12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
+      <c r="H16" s="18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="15" t="s">
         <v>38</v>
       </c>
       <c r="B17" s="6" t="s">
@@ -1029,12 +1642,12 @@
         <f t="shared" si="0"/>
         <v>24.8</v>
       </c>
-      <c r="H17" s="12">
+      <c r="H17" s="18">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="15" t="s">
         <v>42</v>
       </c>
       <c r="B18" s="6" t="s">
@@ -1056,12 +1669,12 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="H18" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
+      <c r="H18" s="18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="15" t="s">
         <v>42</v>
       </c>
       <c r="B19" s="6" t="s">
@@ -1083,12 +1696,12 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="H19" s="12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
+      <c r="H19" s="18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="15" t="s">
         <v>42</v>
       </c>
       <c r="B20" s="6" t="s">
@@ -1110,12 +1723,15 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="H20" s="12">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
+      <c r="H20" s="18">
+        <v>18</v>
+      </c>
+      <c r="I20" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="15" t="s">
         <v>50</v>
       </c>
       <c r="B21" s="6" t="s">
@@ -1137,12 +1753,12 @@
         <f t="shared" si="0"/>
         <v>2.85</v>
       </c>
-      <c r="H21" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
+      <c r="H21" s="18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="15" t="s">
         <v>50</v>
       </c>
       <c r="B22" s="6" t="s">
@@ -1164,12 +1780,12 @@
         <f t="shared" si="0"/>
         <v>2.85</v>
       </c>
-      <c r="H22" s="12">
+      <c r="H22" s="18">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="15" t="s">
         <v>50</v>
       </c>
       <c r="B23" s="6" t="s">
@@ -1191,12 +1807,12 @@
         <f t="shared" si="0"/>
         <v>2.85</v>
       </c>
-      <c r="H23" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="6" t="s">
+      <c r="H23" s="18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="15" t="s">
         <v>58</v>
       </c>
       <c r="B24" s="6" t="s">
@@ -1216,12 +1832,12 @@
         <f t="shared" si="0"/>
         <v>13.26</v>
       </c>
-      <c r="H24" s="12">
+      <c r="H24" s="18">
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="6" t="s">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="15" t="s">
         <v>61</v>
       </c>
       <c r="B25" s="6" t="s">
@@ -1243,12 +1859,12 @@
         <f t="shared" si="0"/>
         <v>4.9400000000000004</v>
       </c>
-      <c r="H25" s="12">
+      <c r="H25" s="18">
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="6" t="s">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="15" t="s">
         <v>65</v>
       </c>
       <c r="B26" s="6"/>
@@ -1263,15 +1879,15 @@
       <c r="G26" s="5">
         <v>0</v>
       </c>
-      <c r="H26" s="13">
+      <c r="H26" s="19">
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="6" t="s">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="B27" s="14" t="s">
+      <c r="B27" s="9" t="s">
         <v>67</v>
       </c>
       <c r="C27" s="6" t="s">
@@ -1290,38 +1906,499 @@
         <f>E27*F27</f>
         <v>6.75</v>
       </c>
-      <c r="H27" s="13">
+      <c r="H27" s="19">
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F29" t="s">
-        <v>70</v>
-      </c>
-      <c r="G29">
-        <f>G6+G7+G8+G9+G10+G11+G12+G13+G14+G15+G16+G17+G18+G19+G20+G21+G22+G23+G24+G25+G26+G27</f>
-        <v>175.32999999999996</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="B28" s="13" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
+      <c r="C28" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3">
-        <v>5</v>
-      </c>
-      <c r="F31" s="3"/>
-      <c r="G31" s="3"/>
-      <c r="H31" s="3">
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="13">
+        <v>12</v>
+      </c>
+      <c r="G28" s="13"/>
+      <c r="H28" s="13">
         <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="B29" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C29" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="D29" s="14"/>
+      <c r="E29" s="14"/>
+      <c r="F29" s="14">
+        <v>20</v>
+      </c>
+      <c r="G29" s="14"/>
+      <c r="H29" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="B30" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="C30" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="13">
+        <v>13</v>
+      </c>
+      <c r="G30" s="13"/>
+      <c r="H30" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="B31" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="C31" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="D31" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="E31" s="14"/>
+      <c r="F31" s="14">
+        <v>25</v>
+      </c>
+      <c r="G31" s="14"/>
+      <c r="H31" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B32" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="C32" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="D32" s="13"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="13">
+        <v>15</v>
+      </c>
+      <c r="G32" s="13"/>
+      <c r="H32" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="B33" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="C33" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="D33" s="14"/>
+      <c r="E33" s="14"/>
+      <c r="F33" s="14">
+        <v>6</v>
+      </c>
+      <c r="G33" s="14"/>
+      <c r="H33" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="B34" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="C34" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="D34" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="E34" s="13"/>
+      <c r="F34" s="13">
+        <v>10</v>
+      </c>
+      <c r="G34" s="13"/>
+      <c r="H34" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="B35" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="C35" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="D35" s="14"/>
+      <c r="E35" s="14"/>
+      <c r="F35" s="14">
+        <v>8</v>
+      </c>
+      <c r="G35" s="14"/>
+      <c r="H35" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="B36" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C36" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="D36" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="E36" s="13"/>
+      <c r="F36" s="13">
+        <v>10</v>
+      </c>
+      <c r="G36" s="13"/>
+      <c r="H36" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="B37" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C37" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="D37" s="14"/>
+      <c r="E37" s="14"/>
+      <c r="F37" s="14">
+        <v>15</v>
+      </c>
+      <c r="G37" s="14"/>
+      <c r="H37" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="B38" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C38" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="D38" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="E38" s="13"/>
+      <c r="F38" s="13">
+        <v>50</v>
+      </c>
+      <c r="G38" s="13"/>
+      <c r="H38" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="B39" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="C39" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="D39" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="E39" s="14"/>
+      <c r="F39" s="14">
+        <v>10</v>
+      </c>
+      <c r="G39" s="14"/>
+      <c r="H39" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="B40" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="C40" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="D40" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="E40" s="13"/>
+      <c r="F40" s="13">
+        <v>10</v>
+      </c>
+      <c r="G40" s="13"/>
+      <c r="H40" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="B41" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="C41" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="D41" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="E41" s="14"/>
+      <c r="F41" s="14">
+        <v>10</v>
+      </c>
+      <c r="G41" s="14"/>
+      <c r="H41" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="B42" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="C42" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="D42" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="E42" s="13"/>
+      <c r="F42" s="13">
+        <v>10</v>
+      </c>
+      <c r="G42" s="13"/>
+      <c r="H42" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="B43" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="C43" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="D43" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="E43" s="14"/>
+      <c r="F43" s="14">
+        <v>10</v>
+      </c>
+      <c r="G43" s="14"/>
+      <c r="H43" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="B44" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="C44" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="D44" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="E44" s="13"/>
+      <c r="F44" s="13">
+        <v>25</v>
+      </c>
+      <c r="G44" s="13"/>
+      <c r="H44" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="B45" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="C45" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="D45" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="E45" s="14"/>
+      <c r="F45" s="14">
+        <v>100</v>
+      </c>
+      <c r="G45" s="14"/>
+      <c r="H45" s="14">
+        <v>2</v>
+      </c>
+      <c r="I45" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="B46" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="C46" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="D46" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="E46" s="13"/>
+      <c r="F46" s="13">
+        <v>10</v>
+      </c>
+      <c r="G46" s="13"/>
+      <c r="H46" s="13"/>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="B47" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="C47" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="D47" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="E47" s="14"/>
+      <c r="F47" s="14">
+        <v>10</v>
+      </c>
+      <c r="G47" s="14"/>
+      <c r="H47" s="14"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="B48" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="C48" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="D48" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="E48" s="13"/>
+      <c r="F48" s="13">
+        <v>2</v>
+      </c>
+      <c r="G48" s="13"/>
+      <c r="H48" s="13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="B49" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="C49" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="D49" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="E49" s="14"/>
+      <c r="F49" s="14">
+        <v>2</v>
+      </c>
+      <c r="G49" s="14"/>
+      <c r="H49" s="14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="B50" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="C50" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="D50" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="E50" s="13"/>
+      <c r="F50" s="13">
+        <v>2</v>
+      </c>
+      <c r="G50" s="13"/>
+      <c r="H50" s="13">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -1330,6 +2407,9 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 

</xml_diff>